<commit_message>
thru logic puzzle 4
</commit_message>
<xml_diff>
--- a/resources/vr_logic_puzzle_sheets.xlsx
+++ b/resources/vr_logic_puzzle_sheets.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakes\BIGJRA.github.io\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E473D5-86DF-41B3-873C-92DB98177B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EAAE7D2-70CE-4B7C-A2E5-66CF511C3ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{7AD40D07-4C0A-4BE5-BACD-E24D5D72854F}"/>
+    <workbookView xWindow="9150" yWindow="162" windowWidth="13686" windowHeight="12048" activeTab="3" xr2:uid="{7AD40D07-4C0A-4BE5-BACD-E24D5D72854F}"/>
   </bookViews>
   <sheets>
     <sheet name="Puzzle1" sheetId="1" r:id="rId1"/>
     <sheet name="Puzzle2" sheetId="2" r:id="rId2"/>
+    <sheet name="Puzzle3" sheetId="3" r:id="rId3"/>
+    <sheet name="Puzzle4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="34">
   <si>
     <t>R</t>
   </si>
@@ -107,6 +109,36 @@
   </si>
   <si>
     <t>Foliat.</t>
+  </si>
+  <si>
+    <t>Luster</t>
+  </si>
+  <si>
+    <t>Slk</t>
+  </si>
+  <si>
+    <t>Vtr</t>
+  </si>
+  <si>
+    <t>Ply</t>
+  </si>
+  <si>
+    <t>Adm</t>
+  </si>
+  <si>
+    <t>Habit</t>
+  </si>
+  <si>
+    <t>Cbc</t>
+  </si>
+  <si>
+    <t>Hex</t>
+  </si>
+  <si>
+    <t>Tbl</t>
+  </si>
+  <si>
+    <t>Cxc</t>
   </si>
 </sst>
 </file>
@@ -184,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -211,6 +243,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -542,15 +577,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3BA17EB-8593-430E-ABC3-CBCB3A67764E}">
-  <dimension ref="A1:R23"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V16" sqref="V16"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="3.26171875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.3125" style="1" customWidth="1"/>
     <col min="2" max="2" width="3.62890625" style="1" customWidth="1"/>
     <col min="3" max="3" width="1.05078125" style="1" customWidth="1"/>
     <col min="4" max="7" width="3.62890625" style="1" customWidth="1"/>
@@ -566,26 +601,26 @@
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="12" t="s">
+      <c r="N1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
       <c r="R1" s="2"/>
     </row>
     <row r="2" spans="1:18" ht="13.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -653,7 +688,7 @@
       <c r="R3" s="2"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="11" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -665,7 +700,7 @@
       <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="11"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
@@ -675,7 +710,7 @@
       <c r="R5" s="2"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="11"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="7" t="s">
         <v>2</v>
       </c>
@@ -685,7 +720,7 @@
       <c r="R6" s="2"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="11"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="8" t="s">
         <v>3</v>
       </c>
@@ -715,7 +750,7 @@
       <c r="R8" s="2"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="11" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -747,7 +782,7 @@
       <c r="R9" s="2"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="11"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
@@ -777,7 +812,7 @@
       <c r="R10" s="2"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="11"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
@@ -807,7 +842,7 @@
       <c r="R11" s="2"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="11"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
@@ -857,7 +892,7 @@
       <c r="R13" s="2"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="1">
@@ -897,7 +932,7 @@
       <c r="R14" s="2"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="11"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="1">
         <v>6</v>
       </c>
@@ -929,7 +964,7 @@
       <c r="R15" s="2"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="11"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="1">
         <v>7</v>
       </c>
@@ -961,7 +996,7 @@
       <c r="R16" s="2"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="11"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="1">
         <v>8</v>
       </c>
@@ -1012,175 +1047,8 @@
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="O19" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="P19" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q19" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="R19" s="2"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="11"/>
-      <c r="B20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="O20" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="P20" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q20" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="R20" s="2"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="11"/>
-      <c r="B21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="O21" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P21" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q21" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="R21" s="2"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="11"/>
-      <c r="B22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="O22" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P22" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q22" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="R22" s="2"/>
-    </row>
-    <row r="23" spans="1:18" ht="6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="4"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="2"/>
-      <c r="R23" s="2"/>
-    </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A19:A22"/>
+  <mergeCells count="6">
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="I1:L1"/>
     <mergeCell ref="N1:Q1"/>
@@ -1195,15 +1063,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AFCF8C9-A186-462A-A474-DD1FB2FAE9CC}">
-  <dimension ref="A1:W28"/>
+  <dimension ref="A1:W23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V16" sqref="V16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="3.26171875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="2.3125" style="3" customWidth="1"/>
     <col min="2" max="2" width="3.62890625" style="3" customWidth="1"/>
     <col min="3" max="3" width="1.05078125" style="3" customWidth="1"/>
     <col min="4" max="7" width="3.62890625" style="3" customWidth="1"/>
@@ -1221,33 +1089,33 @@
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="12" t="s">
+      <c r="N1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
       <c r="R1" s="2"/>
-      <c r="S1" s="12" t="s">
+      <c r="S1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
       <c r="W1" s="2"/>
     </row>
     <row r="2" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -1333,7 +1201,7 @@
       <c r="W3" s="2"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="11" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -1346,7 +1214,7 @@
       <c r="W4" s="2"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="11"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
@@ -1357,7 +1225,7 @@
       <c r="W5" s="2"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="11"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="7" t="s">
         <v>2</v>
       </c>
@@ -1368,7 +1236,7 @@
       <c r="W6" s="2"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="11"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="8" t="s">
         <v>3</v>
       </c>
@@ -1404,7 +1272,7 @@
       <c r="W8" s="2"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="11" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1441,7 +1309,7 @@
       <c r="W9" s="2"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="11"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
@@ -1476,7 +1344,7 @@
       <c r="W10" s="2"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="11"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
@@ -1511,7 +1379,7 @@
       <c r="W11" s="2"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="11"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="3" t="s">
         <v>8</v>
       </c>
@@ -1571,7 +1439,7 @@
       <c r="W13" s="2"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="3">
@@ -1616,7 +1484,7 @@
       <c r="W14" s="2"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="11"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="3">
         <v>6</v>
       </c>
@@ -1653,7 +1521,7 @@
       <c r="W15" s="2"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="11"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="3">
         <v>7</v>
       </c>
@@ -1690,7 +1558,7 @@
       <c r="W16" s="2"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="11"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="3">
         <v>8</v>
       </c>
@@ -1752,7 +1620,7 @@
       <c r="W18" s="2"/>
     </row>
     <row r="19" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="11" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -1797,7 +1665,7 @@
       <c r="W19" s="2"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="10"/>
+      <c r="A20" s="11"/>
       <c r="B20" s="3" t="s">
         <v>12</v>
       </c>
@@ -1836,7 +1704,7 @@
       <c r="W20" s="2"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="10"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="3" t="s">
         <v>13</v>
       </c>
@@ -1879,7 +1747,7 @@
       <c r="W21" s="2"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="10"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="3" t="s">
         <v>14</v>
       </c>
@@ -1942,11 +1810,887 @@
       <c r="V23" s="2"/>
       <c r="W23" s="2"/>
     </row>
-    <row r="24" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="10" t="s">
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A14:A17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E8359EC-AEED-4479-8869-130669781D2A}">
+  <dimension ref="A1:AB28"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G7" sqref="D4:G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="2.3125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="3.62890625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="1.05078125" style="10" customWidth="1"/>
+    <col min="4" max="7" width="3.62890625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="1.05078125" style="10" customWidth="1"/>
+    <col min="9" max="12" width="3.62890625" style="10" customWidth="1"/>
+    <col min="13" max="13" width="1.05078125" style="10" customWidth="1"/>
+    <col min="14" max="17" width="3.62890625" style="10" customWidth="1"/>
+    <col min="18" max="18" width="1.05078125" style="10" customWidth="1"/>
+    <col min="19" max="22" width="3.62890625" style="10" customWidth="1"/>
+    <col min="23" max="23" width="1.05078125" style="10" customWidth="1"/>
+    <col min="24" max="27" width="3.62890625" style="10" customWidth="1"/>
+    <col min="28" max="28" width="1.05078125" style="10" customWidth="1"/>
+    <col min="29" max="16384" width="8.83984375" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" ht="13.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
+      <c r="AB1" s="2"/>
+    </row>
+    <row r="2" spans="1:28" ht="13.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="10">
+        <v>5</v>
+      </c>
+      <c r="J2" s="10">
+        <v>6</v>
+      </c>
+      <c r="K2" s="10">
+        <v>7</v>
+      </c>
+      <c r="L2" s="10">
+        <v>8</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="2"/>
+      <c r="S2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="T2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="U2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="V2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="W2" s="2"/>
+      <c r="X2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y2" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z2" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA2" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB2" s="2"/>
+    </row>
+    <row r="3" spans="1:28" ht="6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="4"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="AB4" s="2"/>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="12"/>
+      <c r="B5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="AB5" s="2"/>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="12"/>
+      <c r="B6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="AB6" s="2"/>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="12"/>
+      <c r="B7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="AB7" s="2"/>
+    </row>
+    <row r="8" spans="1:28" ht="9.3000000000000007" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="9"/>
+      <c r="AB9" s="2"/>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="12"/>
+      <c r="B10" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
+      <c r="Z10" s="9"/>
+      <c r="AA10" s="9"/>
+      <c r="AB10" s="2"/>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="12"/>
+      <c r="B11" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="9"/>
+      <c r="Z11" s="9"/>
+      <c r="AA11" s="9"/>
+      <c r="AB11" s="2"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="12"/>
+      <c r="B12" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="9"/>
+      <c r="AB12" s="2"/>
+    </row>
+    <row r="13" spans="1:28" ht="6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="4"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="10">
+        <v>5</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="M14" s="2"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="9"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="9"/>
+      <c r="Z14" s="9"/>
+      <c r="AA14" s="9"/>
+      <c r="AB14" s="2"/>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="12"/>
+      <c r="B15" s="10">
+        <v>6</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="M15" s="2"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="9"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="9"/>
+      <c r="Y15" s="9"/>
+      <c r="Z15" s="9"/>
+      <c r="AA15" s="9"/>
+      <c r="AB15" s="2"/>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="12"/>
+      <c r="B16" s="10">
+        <v>7</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="M16" s="2"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
+      <c r="AA16" s="9"/>
+      <c r="AB16" s="2"/>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="12"/>
+      <c r="B17" s="10">
+        <v>8</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M17" s="2"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="9"/>
+      <c r="Z17" s="9"/>
+      <c r="AA17" s="9"/>
+      <c r="AB17" s="2"/>
+    </row>
+    <row r="18" spans="1:28" ht="6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="4"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
+      <c r="AB18" s="2"/>
+    </row>
+    <row r="19" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="O19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="P19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="R19" s="2"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="9"/>
+      <c r="Z19" s="9"/>
+      <c r="AA19" s="9"/>
+      <c r="AB19" s="2"/>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="11"/>
+      <c r="B20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O20" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="P20" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q20" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="R20" s="2"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="9"/>
+      <c r="Z20" s="9"/>
+      <c r="AA20" s="9"/>
+      <c r="AB20" s="2"/>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="11"/>
+      <c r="B21" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P21" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q21" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="R21" s="2"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="9"/>
+      <c r="Y21" s="9"/>
+      <c r="Z21" s="9"/>
+      <c r="AA21" s="9"/>
+      <c r="AB21" s="2"/>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="11"/>
+      <c r="B22" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q22" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="R22" s="2"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="2"/>
+      <c r="X22" s="9"/>
+      <c r="Y22" s="9"/>
+      <c r="Z22" s="9"/>
+      <c r="AA22" s="9"/>
+      <c r="AB22" s="2"/>
+    </row>
+    <row r="23" spans="1:28" ht="6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="4"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="2"/>
+      <c r="Z23" s="2"/>
+      <c r="AA23" s="2"/>
+      <c r="AB23" s="2"/>
+    </row>
+    <row r="24" spans="1:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C24" s="2"/>
@@ -1994,10 +2738,15 @@
         <v>16</v>
       </c>
       <c r="W24" s="2"/>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="10"/>
-      <c r="B25" s="3" t="s">
+      <c r="X24" s="9"/>
+      <c r="Y24" s="9"/>
+      <c r="Z24" s="9"/>
+      <c r="AA24" s="9"/>
+      <c r="AB24" s="2"/>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="11"/>
+      <c r="B25" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C25" s="2"/>
@@ -2041,10 +2790,15 @@
         <v>16</v>
       </c>
       <c r="W25" s="2"/>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="10"/>
-      <c r="B26" s="3" t="s">
+      <c r="X25" s="9"/>
+      <c r="Y25" s="9"/>
+      <c r="Z25" s="9"/>
+      <c r="AA25" s="9"/>
+      <c r="AB25" s="2"/>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="11"/>
+      <c r="B26" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C26" s="2"/>
@@ -2092,10 +2846,15 @@
         <v>16</v>
       </c>
       <c r="W26" s="2"/>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="10"/>
-      <c r="B27" s="3" t="s">
+      <c r="X26" s="9"/>
+      <c r="Y26" s="9"/>
+      <c r="Z26" s="9"/>
+      <c r="AA26" s="9"/>
+      <c r="AB26" s="2"/>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="11"/>
+      <c r="B27" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C27" s="2"/>
@@ -2139,8 +2898,13 @@
         <v>17</v>
       </c>
       <c r="W27" s="2"/>
-    </row>
-    <row r="28" spans="1:23" ht="6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="X27" s="9"/>
+      <c r="Y27" s="9"/>
+      <c r="Z27" s="9"/>
+      <c r="AA27" s="9"/>
+      <c r="AB27" s="2"/>
+    </row>
+    <row r="28" spans="1:28" ht="6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="4"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2164,18 +2928,1561 @@
       <c r="U28" s="2"/>
       <c r="V28" s="2"/>
       <c r="W28" s="2"/>
+      <c r="X28" s="2"/>
+      <c r="Y28" s="2"/>
+      <c r="Z28" s="2"/>
+      <c r="AA28" s="2"/>
+      <c r="AB28" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="A14:A17"/>
     <mergeCell ref="A19:A22"/>
-    <mergeCell ref="S1:V1"/>
     <mergeCell ref="A24:A27"/>
+    <mergeCell ref="X1:AA1"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="I1:L1"/>
     <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="S1:V1"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="A9:A12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{763EC4D6-002E-4B7C-99BE-A776762C614B}">
+  <dimension ref="A1:AG33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AI19" sqref="AI19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="2.3125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="3.62890625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="1.05078125" style="10" customWidth="1"/>
+    <col min="4" max="7" width="3.62890625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="1.05078125" style="10" customWidth="1"/>
+    <col min="9" max="12" width="3.62890625" style="10" customWidth="1"/>
+    <col min="13" max="13" width="1.05078125" style="10" customWidth="1"/>
+    <col min="14" max="17" width="3.62890625" style="10" customWidth="1"/>
+    <col min="18" max="18" width="1.05078125" style="10" customWidth="1"/>
+    <col min="19" max="22" width="3.62890625" style="10" customWidth="1"/>
+    <col min="23" max="23" width="1.05078125" style="10" customWidth="1"/>
+    <col min="24" max="27" width="3.62890625" style="10" customWidth="1"/>
+    <col min="28" max="28" width="1.05078125" style="10" customWidth="1"/>
+    <col min="29" max="32" width="3.62890625" style="10" customWidth="1"/>
+    <col min="33" max="33" width="1.05078125" style="10" customWidth="1"/>
+    <col min="34" max="16384" width="8.83984375" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" ht="13.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD1" s="13"/>
+      <c r="AE1" s="13"/>
+      <c r="AF1" s="13"/>
+      <c r="AG1" s="2"/>
+    </row>
+    <row r="2" spans="1:33" ht="13.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="10">
+        <v>5</v>
+      </c>
+      <c r="J2" s="10">
+        <v>6</v>
+      </c>
+      <c r="K2" s="10">
+        <v>7</v>
+      </c>
+      <c r="L2" s="10">
+        <v>8</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="2"/>
+      <c r="S2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="T2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="U2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="V2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="W2" s="2"/>
+      <c r="X2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y2" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z2" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA2" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG2" s="2"/>
+    </row>
+    <row r="3" spans="1:33" ht="6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="4"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AG4" s="2"/>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="12"/>
+      <c r="B5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="AB5" s="2"/>
+      <c r="AG5" s="2"/>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="12"/>
+      <c r="B6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="AB6" s="2"/>
+      <c r="AG6" s="2"/>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="12"/>
+      <c r="B7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="AB7" s="2"/>
+      <c r="AG7" s="2"/>
+    </row>
+    <row r="8" spans="1:33" ht="9.3000000000000007" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2"/>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="9"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="9"/>
+      <c r="AD9" s="9"/>
+      <c r="AE9" s="9"/>
+      <c r="AF9" s="9"/>
+      <c r="AG9" s="2"/>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="12"/>
+      <c r="B10" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
+      <c r="Z10" s="9"/>
+      <c r="AA10" s="9"/>
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="9"/>
+      <c r="AD10" s="9"/>
+      <c r="AE10" s="9"/>
+      <c r="AF10" s="9"/>
+      <c r="AG10" s="2"/>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="12"/>
+      <c r="B11" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="9"/>
+      <c r="Z11" s="9"/>
+      <c r="AA11" s="9"/>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="9"/>
+      <c r="AD11" s="9"/>
+      <c r="AE11" s="9"/>
+      <c r="AF11" s="9"/>
+      <c r="AG11" s="2"/>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="12"/>
+      <c r="B12" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="9"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="9"/>
+      <c r="AD12" s="9"/>
+      <c r="AE12" s="9"/>
+      <c r="AF12" s="9"/>
+      <c r="AG12" s="2"/>
+    </row>
+    <row r="13" spans="1:33" ht="6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="4"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="2"/>
+      <c r="AE13" s="2"/>
+      <c r="AF13" s="2"/>
+      <c r="AG13" s="2"/>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="10">
+        <v>5</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="M14" s="2"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="9"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="9"/>
+      <c r="Z14" s="9"/>
+      <c r="AA14" s="9"/>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="9"/>
+      <c r="AD14" s="9"/>
+      <c r="AE14" s="9"/>
+      <c r="AF14" s="9"/>
+      <c r="AG14" s="2"/>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="12"/>
+      <c r="B15" s="10">
+        <v>6</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="M15" s="2"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="9"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="9"/>
+      <c r="Y15" s="9"/>
+      <c r="Z15" s="9"/>
+      <c r="AA15" s="9"/>
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="9"/>
+      <c r="AD15" s="9"/>
+      <c r="AE15" s="9"/>
+      <c r="AF15" s="9"/>
+      <c r="AG15" s="2"/>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="12"/>
+      <c r="B16" s="10">
+        <v>7</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="M16" s="2"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
+      <c r="AA16" s="9"/>
+      <c r="AB16" s="2"/>
+      <c r="AC16" s="9"/>
+      <c r="AD16" s="9"/>
+      <c r="AE16" s="9"/>
+      <c r="AF16" s="9"/>
+      <c r="AG16" s="2"/>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="12"/>
+      <c r="B17" s="10">
+        <v>8</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M17" s="2"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="9"/>
+      <c r="Z17" s="9"/>
+      <c r="AA17" s="9"/>
+      <c r="AB17" s="2"/>
+      <c r="AC17" s="9"/>
+      <c r="AD17" s="9"/>
+      <c r="AE17" s="9"/>
+      <c r="AF17" s="9"/>
+      <c r="AG17" s="2"/>
+    </row>
+    <row r="18" spans="1:33" ht="6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="4"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
+      <c r="AB18" s="2"/>
+      <c r="AC18" s="2"/>
+      <c r="AD18" s="2"/>
+      <c r="AE18" s="2"/>
+      <c r="AF18" s="2"/>
+      <c r="AG18" s="2"/>
+    </row>
+    <row r="19" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="O19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="P19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="R19" s="2"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="9"/>
+      <c r="Z19" s="9"/>
+      <c r="AA19" s="9"/>
+      <c r="AB19" s="2"/>
+      <c r="AC19" s="9"/>
+      <c r="AD19" s="9"/>
+      <c r="AE19" s="9"/>
+      <c r="AF19" s="9"/>
+      <c r="AG19" s="2"/>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="11"/>
+      <c r="B20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O20" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="P20" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q20" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="R20" s="2"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="9"/>
+      <c r="Z20" s="9"/>
+      <c r="AA20" s="9"/>
+      <c r="AB20" s="2"/>
+      <c r="AC20" s="9"/>
+      <c r="AD20" s="9"/>
+      <c r="AE20" s="9"/>
+      <c r="AF20" s="9"/>
+      <c r="AG20" s="2"/>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="11"/>
+      <c r="B21" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P21" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q21" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="R21" s="2"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="9"/>
+      <c r="Y21" s="9"/>
+      <c r="Z21" s="9"/>
+      <c r="AA21" s="9"/>
+      <c r="AB21" s="2"/>
+      <c r="AC21" s="9"/>
+      <c r="AD21" s="9"/>
+      <c r="AE21" s="9"/>
+      <c r="AF21" s="9"/>
+      <c r="AG21" s="2"/>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="11"/>
+      <c r="B22" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q22" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="R22" s="2"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="2"/>
+      <c r="X22" s="9"/>
+      <c r="Y22" s="9"/>
+      <c r="Z22" s="9"/>
+      <c r="AA22" s="9"/>
+      <c r="AB22" s="2"/>
+      <c r="AC22" s="9"/>
+      <c r="AD22" s="9"/>
+      <c r="AE22" s="9"/>
+      <c r="AF22" s="9"/>
+      <c r="AG22" s="2"/>
+    </row>
+    <row r="23" spans="1:33" ht="6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="4"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="2"/>
+      <c r="Z23" s="2"/>
+      <c r="AA23" s="2"/>
+      <c r="AB23" s="2"/>
+      <c r="AC23" s="2"/>
+      <c r="AD23" s="2"/>
+      <c r="AE23" s="2"/>
+      <c r="AF23" s="2"/>
+      <c r="AG23" s="2"/>
+    </row>
+    <row r="24" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R24" s="2"/>
+      <c r="S24" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="T24" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="U24" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="V24" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="W24" s="2"/>
+      <c r="X24" s="9"/>
+      <c r="Y24" s="9"/>
+      <c r="Z24" s="9"/>
+      <c r="AA24" s="9"/>
+      <c r="AB24" s="2"/>
+      <c r="AC24" s="9"/>
+      <c r="AD24" s="9"/>
+      <c r="AE24" s="9"/>
+      <c r="AF24" s="9"/>
+      <c r="AG24" s="2"/>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="11"/>
+      <c r="B25" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T25" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="U25" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="V25" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="W25" s="2"/>
+      <c r="X25" s="9"/>
+      <c r="Y25" s="9"/>
+      <c r="Z25" s="9"/>
+      <c r="AA25" s="9"/>
+      <c r="AB25" s="2"/>
+      <c r="AC25" s="9"/>
+      <c r="AD25" s="9"/>
+      <c r="AE25" s="9"/>
+      <c r="AF25" s="9"/>
+      <c r="AG25" s="2"/>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="11"/>
+      <c r="B26" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U26" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="V26" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="W26" s="2"/>
+      <c r="X26" s="9"/>
+      <c r="Y26" s="9"/>
+      <c r="Z26" s="9"/>
+      <c r="AA26" s="9"/>
+      <c r="AB26" s="2"/>
+      <c r="AC26" s="9"/>
+      <c r="AD26" s="9"/>
+      <c r="AE26" s="9"/>
+      <c r="AF26" s="9"/>
+      <c r="AG26" s="2"/>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="11"/>
+      <c r="B27" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="V27" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="W27" s="2"/>
+      <c r="X27" s="9"/>
+      <c r="Y27" s="9"/>
+      <c r="Z27" s="9"/>
+      <c r="AA27" s="9"/>
+      <c r="AB27" s="2"/>
+      <c r="AC27" s="9"/>
+      <c r="AD27" s="9"/>
+      <c r="AE27" s="9"/>
+      <c r="AF27" s="9"/>
+      <c r="AG27" s="2"/>
+    </row>
+    <row r="28" spans="1:33" ht="6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="4"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+      <c r="W28" s="2"/>
+      <c r="X28" s="2"/>
+      <c r="Y28" s="2"/>
+      <c r="Z28" s="2"/>
+      <c r="AA28" s="2"/>
+      <c r="AB28" s="2"/>
+      <c r="AC28" s="2"/>
+      <c r="AD28" s="2"/>
+      <c r="AE28" s="2"/>
+      <c r="AF28" s="2"/>
+      <c r="AG28" s="2"/>
+    </row>
+    <row r="29" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="O29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2"/>
+      <c r="V29" s="2"/>
+      <c r="W29" s="2"/>
+      <c r="X29" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y29" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z29" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA29" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB29" s="2"/>
+      <c r="AC29" s="9"/>
+      <c r="AD29" s="9"/>
+      <c r="AE29" s="9"/>
+      <c r="AF29" s="9"/>
+      <c r="AG29" s="2"/>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="11"/>
+      <c r="B30" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P30" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q30" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="2"/>
+      <c r="X30" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y30" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z30" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA30" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB30" s="2"/>
+      <c r="AC30" s="9"/>
+      <c r="AD30" s="9"/>
+      <c r="AE30" s="9"/>
+      <c r="AF30" s="9"/>
+      <c r="AG30" s="2"/>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="11"/>
+      <c r="B31" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P31" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R31" s="2"/>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+      <c r="U31" s="2"/>
+      <c r="V31" s="2"/>
+      <c r="W31" s="2"/>
+      <c r="X31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z31" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA31" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB31" s="2"/>
+      <c r="AC31" s="9"/>
+      <c r="AD31" s="9"/>
+      <c r="AE31" s="9"/>
+      <c r="AF31" s="9"/>
+      <c r="AG31" s="2"/>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="11"/>
+      <c r="B32" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q32" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R32" s="2"/>
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2"/>
+      <c r="V32" s="2"/>
+      <c r="W32" s="2"/>
+      <c r="X32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA32" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB32" s="2"/>
+      <c r="AC32" s="9"/>
+      <c r="AD32" s="9"/>
+      <c r="AE32" s="9"/>
+      <c r="AF32" s="9"/>
+      <c r="AG32" s="2"/>
+    </row>
+    <row r="33" spans="1:33" ht="6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="4"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2"/>
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+      <c r="W33" s="2"/>
+      <c r="X33" s="2"/>
+      <c r="Y33" s="2"/>
+      <c r="Z33" s="2"/>
+      <c r="AA33" s="2"/>
+      <c r="AB33" s="2"/>
+      <c r="AC33" s="2"/>
+      <c r="AD33" s="2"/>
+      <c r="AE33" s="2"/>
+      <c r="AF33" s="2"/>
+      <c r="AG33" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A9:A12"/>
     <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="AC1:AF1"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="X1:AA1"/>
+    <mergeCell ref="A4:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>